<commit_message>
Released RDB V1.7. Updated FTINT PCB with DNF components
</commit_message>
<xml_diff>
--- a/P-FTINT-1-1/P-FTINT-1-1 (BoM).xlsx
+++ b/P-FTINT-1-1/P-FTINT-1-1 (BoM).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevMSR\4x4\TFVC\BlancaHW\Interfaces\P-FTINT-1-1\Altium\Project Outputs for P-FTINT-1-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\cust-Hardware\ReferenceDesigns\P-FTINT-1-1\Altium\Project Outputs for P-FTINT-1-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF25AA5-9801-4570-9355-E3EA74B96215}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{569A5B7F-585E-407F-B455-D15D9D5EFA53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7815" yWindow="3885" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -62,25 +62,22 @@
     <t>Report Time:</t>
   </si>
   <si>
-    <t xml:space="preserve">                     Microsoft AI and Research</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    MICROSOFT CONFIDENTIAL</t>
-  </si>
-  <si>
-    <t>P-FTINT-1-1.PcbDoc</t>
+    <t xml:space="preserve">                       Microsoft Azure Sphere</t>
   </si>
   <si>
     <t>P-FTINT-1-1.PrjPCB</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>09/08/2019</t>
-  </si>
-  <si>
-    <t>16:43</t>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>22/04/2021</t>
+  </si>
+  <si>
+    <t>17:07</t>
   </si>
   <si>
     <t>Designator</t>
@@ -89,18 +86,9 @@
     <t>C1</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
-    <t>J2</t>
-  </si>
-  <si>
     <t>J3, J4</t>
   </si>
   <si>
@@ -110,10 +98,7 @@
     <t>R1, R2, R4, R5, R6, R7, R8</t>
   </si>
   <si>
-    <t>R3, R9, R10, R11, R12</t>
-  </si>
-  <si>
-    <t>R13, R14</t>
+    <t>R3, R9, R10, R11</t>
   </si>
   <si>
     <t>R15, R16</t>
@@ -125,27 +110,15 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>#Column Name Error:' Fitted</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
     <t>0.1uF</t>
   </si>
   <si>
-    <t>SML-D12U</t>
-  </si>
-  <si>
-    <t>SML-D12P</t>
-  </si>
-  <si>
     <t>FTSH-105-01-F-DV-K</t>
   </si>
   <si>
-    <t>MOLEX-0022284020</t>
-  </si>
-  <si>
     <t>FT4232H-56QMINIMDL</t>
   </si>
   <si>
@@ -155,9 +128,6 @@
     <t>4K7</t>
   </si>
   <si>
-    <t>604R</t>
-  </si>
-  <si>
     <t>2K2</t>
   </si>
   <si>
@@ -170,18 +140,9 @@
     <t>CAP CER 0.1UF 25V X7R 0603</t>
   </si>
   <si>
-    <t>1.6 x 0.8 x 0.55mm (0603) LED 620nm Red</t>
-  </si>
-  <si>
-    <t>1.6 x 0.8 x 0.55mm (0603) LED 560nm Green</t>
-  </si>
-  <si>
     <t>CONN HEADER 10POS DUAL .05" SMD</t>
   </si>
   <si>
-    <t>CONN HEADER 2POS .100 VERT TIN</t>
-  </si>
-  <si>
     <t>CONN HEADER 10POS .100" STR GOLD</t>
   </si>
   <si>
@@ -194,9 +155,6 @@
     <t>RES SMD 4.7K OHM 5% 1/10W 0603</t>
   </si>
   <si>
-    <t>RES SMD 604 OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
     <t>RES SMD 2.2K OHM 5% 1/10W 0603</t>
   </si>
   <si>
@@ -218,18 +176,9 @@
     <t>445-5667-1-ND</t>
   </si>
   <si>
-    <t>511-1580-1-ND</t>
-  </si>
-  <si>
-    <t>511-1579-1-ND</t>
-  </si>
-  <si>
     <t>SAM8796-ND</t>
   </si>
   <si>
-    <t>WM50014-02-ND</t>
-  </si>
-  <si>
     <t>WM8141-ND</t>
   </si>
   <si>
@@ -239,9 +188,6 @@
     <t>P4.7KGCT-ND</t>
   </si>
   <si>
-    <t>P604HCT-ND</t>
-  </si>
-  <si>
     <t>P2.2KGCT-ND</t>
   </si>
   <si>
@@ -254,9 +200,6 @@
     <t>TDK</t>
   </si>
   <si>
-    <t>Rohm Semiconductor</t>
-  </si>
-  <si>
     <t>Samtec Inc.</t>
   </si>
   <si>
@@ -278,19 +221,10 @@
     <t>CGA3E2X7R1E104K080AA</t>
   </si>
   <si>
-    <t>SML-D12U8WT86</t>
-  </si>
-  <si>
-    <t>SML-D12P8WT86</t>
-  </si>
-  <si>
     <t>ERJ-3GEYJ330V</t>
   </si>
   <si>
     <t>ERJ-3GEYJ472V</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF6040V</t>
   </si>
   <si>
     <t>ERJ-3GEYJ222V</t>
@@ -691,9 +625,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -730,6 +661,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1082,28 +1014,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CB27"/>
+  <dimension ref="A1:CA23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="34.73046875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="33.46484375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="39.1328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.86328125" style="2" customWidth="1"/>
-    <col min="9" max="10" width="36.3984375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.86328125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.1328125" style="2"/>
+    <col min="8" max="8" width="25.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:79" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17"/>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1114,9 +1046,8 @@
       <c r="H1" s="25"/>
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-    </row>
-    <row r="2" spans="1:80" ht="34.9" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:79" ht="38.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
@@ -1129,9 +1060,8 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
       <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-    </row>
-    <row r="3" spans="1:80" ht="15.4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:79" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="31"/>
       <c r="C3" s="32"/>
@@ -1139,16 +1069,15 @@
         <v>1</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="33"/>
       <c r="H3" s="33"/>
       <c r="I3" s="33"/>
       <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-    </row>
-    <row r="4" spans="1:80" ht="15.4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:79" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="31"/>
       <c r="C4" s="32"/>
@@ -1156,16 +1085,15 @@
         <v>4</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="34"/>
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
       <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-    </row>
-    <row r="5" spans="1:80" ht="15.4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:79" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
@@ -1173,117 +1101,108 @@
         <v>5</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" s="34"/>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
       <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-    </row>
-    <row r="6" spans="1:80" ht="16.5" x14ac:dyDescent="0.6">
+    </row>
+    <row r="6" spans="1:79" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="51" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="35">
-        <v>10</v>
+      <c r="E6" s="54" t="s">
+        <v>13</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="33"/>
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-    </row>
-    <row r="7" spans="1:80" ht="16.5" x14ac:dyDescent="0.6">
+    </row>
+    <row r="7" spans="1:79" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="31" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="41"/>
+        <v>14</v>
+      </c>
+      <c r="F7" s="40"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
       <c r="I7" s="33"/>
       <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-    </row>
-    <row r="8" spans="1:80" ht="16.5" x14ac:dyDescent="0.6">
+    </row>
+    <row r="8" spans="1:79" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
-      <c r="B8" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="42"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="31" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="39"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="33"/>
       <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-    </row>
-    <row r="9" spans="1:80" ht="15.4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:79" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="34"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="34"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="39"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="33"/>
       <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-    </row>
-    <row r="10" spans="1:80" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:79" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
-      <c r="B10" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="45" t="s">
-        <v>30</v>
+      <c r="B10" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>25</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="K10" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="44" t="s">
         <v>3</v>
       </c>
+      <c r="K10" s="20"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="20"/>
@@ -1352,38 +1271,37 @@
       <c r="BY10" s="20"/>
       <c r="BZ10" s="20"/>
       <c r="CA10" s="20"/>
-      <c r="CB10" s="20"/>
-    </row>
-    <row r="11" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="48">
+    </row>
+    <row r="11" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="47">
         <v>1</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="J11" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="K11" s="49">
-        <f t="shared" ref="K11:K22" si="0">$E$6*C11</f>
-        <v>10</v>
-      </c>
+      <c r="D11" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="48">
+        <f>$E$6*C11</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="21"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
@@ -1452,38 +1370,37 @@
       <c r="BY11" s="21"/>
       <c r="BZ11" s="21"/>
       <c r="CA11" s="21"/>
-      <c r="CB11" s="21"/>
-    </row>
-    <row r="12" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="48">
+    </row>
+    <row r="12" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="47">
         <v>1</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="J12" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="K12" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+      <c r="D12" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="48">
+        <f>$E$6*C12</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="21"/>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
@@ -1552,38 +1469,37 @@
       <c r="BY12" s="21"/>
       <c r="BZ12" s="21"/>
       <c r="CA12" s="21"/>
-      <c r="CB12" s="21"/>
-    </row>
-    <row r="13" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="48">
-        <v>1</v>
-      </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="K13" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+    </row>
+    <row r="13" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="47">
+        <v>2</v>
+      </c>
+      <c r="D13" s="47">
+        <v>901310765</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="48">
+        <v>901310765</v>
+      </c>
+      <c r="J13" s="48">
+        <f>$E$6*C13</f>
+        <v>2</v>
+      </c>
+      <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
@@ -1652,38 +1568,37 @@
       <c r="BY13" s="21"/>
       <c r="BZ13" s="21"/>
       <c r="CA13" s="21"/>
-      <c r="CB13" s="21"/>
-    </row>
-    <row r="14" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="48">
+    </row>
+    <row r="14" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="47">
         <v>1</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="49" t="s">
+      <c r="D14" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="48">
+        <v>2535452</v>
+      </c>
+      <c r="H14" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="I14" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="J14" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="K14" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+      <c r="I14" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="48">
+        <f>$E$6*C14</f>
+        <v>1</v>
+      </c>
+      <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
@@ -1752,38 +1667,37 @@
       <c r="BY14" s="21"/>
       <c r="BZ14" s="21"/>
       <c r="CA14" s="21"/>
-      <c r="CB14" s="21"/>
-    </row>
-    <row r="15" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="48">
-        <v>1</v>
-      </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="J15" s="50">
-        <v>22284020</v>
-      </c>
-      <c r="K15" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+    </row>
+    <row r="15" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="47">
+        <v>7</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="48">
+        <f>$E$6*C15</f>
+        <v>7</v>
+      </c>
+      <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
@@ -1852,38 +1766,37 @@
       <c r="BY15" s="21"/>
       <c r="BZ15" s="21"/>
       <c r="CA15" s="21"/>
-      <c r="CB15" s="21"/>
-    </row>
-    <row r="16" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="48">
-        <v>2</v>
-      </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="50">
-        <v>901310765</v>
-      </c>
-      <c r="F16" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="J16" s="50">
-        <v>901310765</v>
-      </c>
-      <c r="K16" s="49">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
+    </row>
+    <row r="16" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="47">
+        <v>4</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="48">
+        <f>$E$6*C16</f>
+        <v>4</v>
+      </c>
+      <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
@@ -1952,38 +1865,37 @@
       <c r="BY16" s="21"/>
       <c r="BZ16" s="21"/>
       <c r="CA16" s="21"/>
-      <c r="CB16" s="21"/>
-    </row>
-    <row r="17" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="48">
-        <v>1</v>
-      </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="49" t="s">
+    </row>
+    <row r="17" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="47">
+        <v>2</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="H17" s="50">
-        <v>2535452</v>
-      </c>
-      <c r="I17" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="J17" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+      <c r="I17" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" s="48">
+        <f>$E$6*C17</f>
+        <v>2</v>
+      </c>
+      <c r="K17" s="21"/>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
@@ -2052,38 +1964,37 @@
       <c r="BY17" s="21"/>
       <c r="BZ17" s="21"/>
       <c r="CA17" s="21"/>
-      <c r="CB17" s="21"/>
-    </row>
-    <row r="18" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="48">
-        <v>7</v>
-      </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="J18" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="K18" s="49">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
+    </row>
+    <row r="18" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="47">
+        <v>1</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="48">
+        <f>$E$6*C18</f>
+        <v>1</v>
+      </c>
+      <c r="K18" s="21"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
@@ -2152,453 +2063,50 @@
       <c r="BY18" s="21"/>
       <c r="BZ18" s="21"/>
       <c r="CA18" s="21"/>
-      <c r="CB18" s="21"/>
-    </row>
-    <row r="19" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="48">
-        <v>5</v>
-      </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="I19" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="J19" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="K19" s="49">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="21"/>
-      <c r="AB19" s="21"/>
-      <c r="AC19" s="21"/>
-      <c r="AD19" s="21"/>
-      <c r="AE19" s="21"/>
-      <c r="AF19" s="21"/>
-      <c r="AG19" s="21"/>
-      <c r="AH19" s="21"/>
-      <c r="AI19" s="21"/>
-      <c r="AJ19" s="21"/>
-      <c r="AK19" s="21"/>
-      <c r="AL19" s="21"/>
-      <c r="AM19" s="21"/>
-      <c r="AN19" s="21"/>
-      <c r="AO19" s="21"/>
-      <c r="AP19" s="21"/>
-      <c r="AQ19" s="21"/>
-      <c r="AR19" s="21"/>
-      <c r="AS19" s="21"/>
-      <c r="AT19" s="21"/>
-      <c r="AU19" s="21"/>
-      <c r="AV19" s="21"/>
-      <c r="AW19" s="21"/>
-      <c r="AX19" s="21"/>
-      <c r="AY19" s="21"/>
-      <c r="AZ19" s="21"/>
-      <c r="BA19" s="21"/>
-      <c r="BB19" s="21"/>
-      <c r="BC19" s="21"/>
-      <c r="BD19" s="21"/>
-      <c r="BE19" s="21"/>
-      <c r="BF19" s="21"/>
-      <c r="BG19" s="21"/>
-      <c r="BH19" s="21"/>
-      <c r="BI19" s="21"/>
-      <c r="BJ19" s="21"/>
-      <c r="BK19" s="21"/>
-      <c r="BL19" s="21"/>
-      <c r="BM19" s="21"/>
-      <c r="BN19" s="21"/>
-      <c r="BO19" s="21"/>
-      <c r="BP19" s="21"/>
-      <c r="BQ19" s="21"/>
-      <c r="BR19" s="21"/>
-      <c r="BS19" s="21"/>
-      <c r="BT19" s="21"/>
-      <c r="BU19" s="21"/>
-      <c r="BV19" s="21"/>
-      <c r="BW19" s="21"/>
-      <c r="BX19" s="21"/>
-      <c r="BY19" s="21"/>
-      <c r="BZ19" s="21"/>
-      <c r="CA19" s="21"/>
-      <c r="CB19" s="21"/>
-    </row>
-    <row r="20" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="48">
-        <v>2</v>
-      </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="J20" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="K20" s="49">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="21"/>
-      <c r="AC20" s="21"/>
-      <c r="AD20" s="21"/>
-      <c r="AE20" s="21"/>
-      <c r="AF20" s="21"/>
-      <c r="AG20" s="21"/>
-      <c r="AH20" s="21"/>
-      <c r="AI20" s="21"/>
-      <c r="AJ20" s="21"/>
-      <c r="AK20" s="21"/>
-      <c r="AL20" s="21"/>
-      <c r="AM20" s="21"/>
-      <c r="AN20" s="21"/>
-      <c r="AO20" s="21"/>
-      <c r="AP20" s="21"/>
-      <c r="AQ20" s="21"/>
-      <c r="AR20" s="21"/>
-      <c r="AS20" s="21"/>
-      <c r="AT20" s="21"/>
-      <c r="AU20" s="21"/>
-      <c r="AV20" s="21"/>
-      <c r="AW20" s="21"/>
-      <c r="AX20" s="21"/>
-      <c r="AY20" s="21"/>
-      <c r="AZ20" s="21"/>
-      <c r="BA20" s="21"/>
-      <c r="BB20" s="21"/>
-      <c r="BC20" s="21"/>
-      <c r="BD20" s="21"/>
-      <c r="BE20" s="21"/>
-      <c r="BF20" s="21"/>
-      <c r="BG20" s="21"/>
-      <c r="BH20" s="21"/>
-      <c r="BI20" s="21"/>
-      <c r="BJ20" s="21"/>
-      <c r="BK20" s="21"/>
-      <c r="BL20" s="21"/>
-      <c r="BM20" s="21"/>
-      <c r="BN20" s="21"/>
-      <c r="BO20" s="21"/>
-      <c r="BP20" s="21"/>
-      <c r="BQ20" s="21"/>
-      <c r="BR20" s="21"/>
-      <c r="BS20" s="21"/>
-      <c r="BT20" s="21"/>
-      <c r="BU20" s="21"/>
-      <c r="BV20" s="21"/>
-      <c r="BW20" s="21"/>
-      <c r="BX20" s="21"/>
-      <c r="BY20" s="21"/>
-      <c r="BZ20" s="21"/>
-      <c r="CA20" s="21"/>
-      <c r="CB20" s="21"/>
-    </row>
-    <row r="21" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="48">
-        <v>2</v>
-      </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="J21" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="K21" s="49">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="21"/>
-      <c r="AB21" s="21"/>
-      <c r="AC21" s="21"/>
-      <c r="AD21" s="21"/>
-      <c r="AE21" s="21"/>
-      <c r="AF21" s="21"/>
-      <c r="AG21" s="21"/>
-      <c r="AH21" s="21"/>
-      <c r="AI21" s="21"/>
-      <c r="AJ21" s="21"/>
-      <c r="AK21" s="21"/>
-      <c r="AL21" s="21"/>
-      <c r="AM21" s="21"/>
-      <c r="AN21" s="21"/>
-      <c r="AO21" s="21"/>
-      <c r="AP21" s="21"/>
-      <c r="AQ21" s="21"/>
-      <c r="AR21" s="21"/>
-      <c r="AS21" s="21"/>
-      <c r="AT21" s="21"/>
-      <c r="AU21" s="21"/>
-      <c r="AV21" s="21"/>
-      <c r="AW21" s="21"/>
-      <c r="AX21" s="21"/>
-      <c r="AY21" s="21"/>
-      <c r="AZ21" s="21"/>
-      <c r="BA21" s="21"/>
-      <c r="BB21" s="21"/>
-      <c r="BC21" s="21"/>
-      <c r="BD21" s="21"/>
-      <c r="BE21" s="21"/>
-      <c r="BF21" s="21"/>
-      <c r="BG21" s="21"/>
-      <c r="BH21" s="21"/>
-      <c r="BI21" s="21"/>
-      <c r="BJ21" s="21"/>
-      <c r="BK21" s="21"/>
-      <c r="BL21" s="21"/>
-      <c r="BM21" s="21"/>
-      <c r="BN21" s="21"/>
-      <c r="BO21" s="21"/>
-      <c r="BP21" s="21"/>
-      <c r="BQ21" s="21"/>
-      <c r="BR21" s="21"/>
-      <c r="BS21" s="21"/>
-      <c r="BT21" s="21"/>
-      <c r="BU21" s="21"/>
-      <c r="BV21" s="21"/>
-      <c r="BW21" s="21"/>
-      <c r="BX21" s="21"/>
-      <c r="BY21" s="21"/>
-      <c r="BZ21" s="21"/>
-      <c r="CA21" s="21"/>
-      <c r="CB21" s="21"/>
-    </row>
-    <row r="22" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="48">
-        <v>1</v>
-      </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="I22" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="J22" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="K22" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="21"/>
-      <c r="AD22" s="21"/>
-      <c r="AE22" s="21"/>
-      <c r="AF22" s="21"/>
-      <c r="AG22" s="21"/>
-      <c r="AH22" s="21"/>
-      <c r="AI22" s="21"/>
-      <c r="AJ22" s="21"/>
-      <c r="AK22" s="21"/>
-      <c r="AL22" s="21"/>
-      <c r="AM22" s="21"/>
-      <c r="AN22" s="21"/>
-      <c r="AO22" s="21"/>
-      <c r="AP22" s="21"/>
-      <c r="AQ22" s="21"/>
-      <c r="AR22" s="21"/>
-      <c r="AS22" s="21"/>
-      <c r="AT22" s="21"/>
-      <c r="AU22" s="21"/>
-      <c r="AV22" s="21"/>
-      <c r="AW22" s="21"/>
-      <c r="AX22" s="21"/>
-      <c r="AY22" s="21"/>
-      <c r="AZ22" s="21"/>
-      <c r="BA22" s="21"/>
-      <c r="BB22" s="21"/>
-      <c r="BC22" s="21"/>
-      <c r="BD22" s="21"/>
-      <c r="BE22" s="21"/>
-      <c r="BF22" s="21"/>
-      <c r="BG22" s="21"/>
-      <c r="BH22" s="21"/>
-      <c r="BI22" s="21"/>
-      <c r="BJ22" s="21"/>
-      <c r="BK22" s="21"/>
-      <c r="BL22" s="21"/>
-      <c r="BM22" s="21"/>
-      <c r="BN22" s="21"/>
-      <c r="BO22" s="21"/>
-      <c r="BP22" s="21"/>
-      <c r="BQ22" s="21"/>
-      <c r="BR22" s="21"/>
-      <c r="BS22" s="21"/>
-      <c r="BT22" s="21"/>
-      <c r="BU22" s="21"/>
-      <c r="BV22" s="21"/>
-      <c r="BW22" s="21"/>
-      <c r="BX22" s="21"/>
-      <c r="BY22" s="21"/>
-      <c r="BZ22" s="21"/>
-      <c r="CA22" s="21"/>
-      <c r="CB22" s="21"/>
-    </row>
-    <row r="23" spans="1:80" ht="14.65" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="13"/>
-      <c r="C23" s="14">
-        <f>SUM(C11:C22)</f>
-        <v>25</v>
-      </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="1:80" customFormat="1" ht="13.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="E24" s="5" t="s">
+    </row>
+    <row r="19" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="14">
+        <f>SUM(C11:C18)</f>
+        <v>19</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:79" customFormat="1" ht="13.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E20" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:80" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:80" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:80" ht="15.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="9"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="8"/>
+    <row r="21" spans="1:79" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:79" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:79" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2609,4 +2117,10 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Released RDB V1.7. Updated FTINT PCB with DNF components (#21)
* Released RDB V1.7. Updated FTINT PCB with DNF components

* Update README.md

Co-authored-by: dheram <rdheeraj@microsoft.com>
Co-authored-by: James Scott <jws@microsoft.com>
</commit_message>
<xml_diff>
--- a/P-FTINT-1-1/P-FTINT-1-1 (BoM).xlsx
+++ b/P-FTINT-1-1/P-FTINT-1-1 (BoM).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevMSR\4x4\TFVC\BlancaHW\Interfaces\P-FTINT-1-1\Altium\Project Outputs for P-FTINT-1-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\cust-Hardware\ReferenceDesigns\P-FTINT-1-1\Altium\Project Outputs for P-FTINT-1-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF25AA5-9801-4570-9355-E3EA74B96215}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{569A5B7F-585E-407F-B455-D15D9D5EFA53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7815" yWindow="3885" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -62,25 +62,22 @@
     <t>Report Time:</t>
   </si>
   <si>
-    <t xml:space="preserve">                     Microsoft AI and Research</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    MICROSOFT CONFIDENTIAL</t>
-  </si>
-  <si>
-    <t>P-FTINT-1-1.PcbDoc</t>
+    <t xml:space="preserve">                       Microsoft Azure Sphere</t>
   </si>
   <si>
     <t>P-FTINT-1-1.PrjPCB</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>09/08/2019</t>
-  </si>
-  <si>
-    <t>16:43</t>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>22/04/2021</t>
+  </si>
+  <si>
+    <t>17:07</t>
   </si>
   <si>
     <t>Designator</t>
@@ -89,18 +86,9 @@
     <t>C1</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
-    <t>J2</t>
-  </si>
-  <si>
     <t>J3, J4</t>
   </si>
   <si>
@@ -110,10 +98,7 @@
     <t>R1, R2, R4, R5, R6, R7, R8</t>
   </si>
   <si>
-    <t>R3, R9, R10, R11, R12</t>
-  </si>
-  <si>
-    <t>R13, R14</t>
+    <t>R3, R9, R10, R11</t>
   </si>
   <si>
     <t>R15, R16</t>
@@ -125,27 +110,15 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>#Column Name Error:' Fitted</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
     <t>0.1uF</t>
   </si>
   <si>
-    <t>SML-D12U</t>
-  </si>
-  <si>
-    <t>SML-D12P</t>
-  </si>
-  <si>
     <t>FTSH-105-01-F-DV-K</t>
   </si>
   <si>
-    <t>MOLEX-0022284020</t>
-  </si>
-  <si>
     <t>FT4232H-56QMINIMDL</t>
   </si>
   <si>
@@ -155,9 +128,6 @@
     <t>4K7</t>
   </si>
   <si>
-    <t>604R</t>
-  </si>
-  <si>
     <t>2K2</t>
   </si>
   <si>
@@ -170,18 +140,9 @@
     <t>CAP CER 0.1UF 25V X7R 0603</t>
   </si>
   <si>
-    <t>1.6 x 0.8 x 0.55mm (0603) LED 620nm Red</t>
-  </si>
-  <si>
-    <t>1.6 x 0.8 x 0.55mm (0603) LED 560nm Green</t>
-  </si>
-  <si>
     <t>CONN HEADER 10POS DUAL .05" SMD</t>
   </si>
   <si>
-    <t>CONN HEADER 2POS .100 VERT TIN</t>
-  </si>
-  <si>
     <t>CONN HEADER 10POS .100" STR GOLD</t>
   </si>
   <si>
@@ -194,9 +155,6 @@
     <t>RES SMD 4.7K OHM 5% 1/10W 0603</t>
   </si>
   <si>
-    <t>RES SMD 604 OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
     <t>RES SMD 2.2K OHM 5% 1/10W 0603</t>
   </si>
   <si>
@@ -218,18 +176,9 @@
     <t>445-5667-1-ND</t>
   </si>
   <si>
-    <t>511-1580-1-ND</t>
-  </si>
-  <si>
-    <t>511-1579-1-ND</t>
-  </si>
-  <si>
     <t>SAM8796-ND</t>
   </si>
   <si>
-    <t>WM50014-02-ND</t>
-  </si>
-  <si>
     <t>WM8141-ND</t>
   </si>
   <si>
@@ -239,9 +188,6 @@
     <t>P4.7KGCT-ND</t>
   </si>
   <si>
-    <t>P604HCT-ND</t>
-  </si>
-  <si>
     <t>P2.2KGCT-ND</t>
   </si>
   <si>
@@ -254,9 +200,6 @@
     <t>TDK</t>
   </si>
   <si>
-    <t>Rohm Semiconductor</t>
-  </si>
-  <si>
     <t>Samtec Inc.</t>
   </si>
   <si>
@@ -278,19 +221,10 @@
     <t>CGA3E2X7R1E104K080AA</t>
   </si>
   <si>
-    <t>SML-D12U8WT86</t>
-  </si>
-  <si>
-    <t>SML-D12P8WT86</t>
-  </si>
-  <si>
     <t>ERJ-3GEYJ330V</t>
   </si>
   <si>
     <t>ERJ-3GEYJ472V</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF6040V</t>
   </si>
   <si>
     <t>ERJ-3GEYJ222V</t>
@@ -691,9 +625,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -730,6 +661,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1082,28 +1014,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CB27"/>
+  <dimension ref="A1:CA23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="34.73046875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="33.46484375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="39.1328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="33.265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.86328125" style="2" customWidth="1"/>
-    <col min="9" max="10" width="36.3984375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.86328125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.1328125" style="2"/>
+    <col min="8" max="8" width="25.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:79" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17"/>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1114,9 +1046,8 @@
       <c r="H1" s="25"/>
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-    </row>
-    <row r="2" spans="1:80" ht="34.9" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:79" ht="38.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
@@ -1129,9 +1060,8 @@
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
       <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-    </row>
-    <row r="3" spans="1:80" ht="15.4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:79" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="31"/>
       <c r="C3" s="32"/>
@@ -1139,16 +1069,15 @@
         <v>1</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="33"/>
       <c r="H3" s="33"/>
       <c r="I3" s="33"/>
       <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-    </row>
-    <row r="4" spans="1:80" ht="15.4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:79" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="31"/>
       <c r="C4" s="32"/>
@@ -1156,16 +1085,15 @@
         <v>4</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="34"/>
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
       <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-    </row>
-    <row r="5" spans="1:80" ht="15.4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:79" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
@@ -1173,117 +1101,108 @@
         <v>5</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" s="34"/>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
       <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-    </row>
-    <row r="6" spans="1:80" ht="16.5" x14ac:dyDescent="0.6">
+    </row>
+    <row r="6" spans="1:79" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="51" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="35">
-        <v>10</v>
+      <c r="E6" s="54" t="s">
+        <v>13</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="33"/>
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-    </row>
-    <row r="7" spans="1:80" ht="16.5" x14ac:dyDescent="0.6">
+    </row>
+    <row r="7" spans="1:79" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="31" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="41"/>
+        <v>14</v>
+      </c>
+      <c r="F7" s="40"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
       <c r="I7" s="33"/>
       <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-    </row>
-    <row r="8" spans="1:80" ht="16.5" x14ac:dyDescent="0.6">
+    </row>
+    <row r="8" spans="1:79" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
-      <c r="B8" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="42"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="31" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="39"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="33"/>
       <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-    </row>
-    <row r="9" spans="1:80" ht="15.4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:79" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="34"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="34"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="39"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="33"/>
       <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-    </row>
-    <row r="10" spans="1:80" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:79" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
-      <c r="B10" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="45" t="s">
-        <v>30</v>
+      <c r="B10" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>25</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="K10" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="44" t="s">
         <v>3</v>
       </c>
+      <c r="K10" s="20"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="20"/>
@@ -1352,38 +1271,37 @@
       <c r="BY10" s="20"/>
       <c r="BZ10" s="20"/>
       <c r="CA10" s="20"/>
-      <c r="CB10" s="20"/>
-    </row>
-    <row r="11" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="48">
+    </row>
+    <row r="11" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="47">
         <v>1</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="J11" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="K11" s="49">
-        <f t="shared" ref="K11:K22" si="0">$E$6*C11</f>
-        <v>10</v>
-      </c>
+      <c r="D11" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="48">
+        <f>$E$6*C11</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="21"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
@@ -1452,38 +1370,37 @@
       <c r="BY11" s="21"/>
       <c r="BZ11" s="21"/>
       <c r="CA11" s="21"/>
-      <c r="CB11" s="21"/>
-    </row>
-    <row r="12" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="48">
+    </row>
+    <row r="12" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="47">
         <v>1</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="J12" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="K12" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+      <c r="D12" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="48">
+        <f>$E$6*C12</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="21"/>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
@@ -1552,38 +1469,37 @@
       <c r="BY12" s="21"/>
       <c r="BZ12" s="21"/>
       <c r="CA12" s="21"/>
-      <c r="CB12" s="21"/>
-    </row>
-    <row r="13" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="48">
-        <v>1</v>
-      </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="K13" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+    </row>
+    <row r="13" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="47">
+        <v>2</v>
+      </c>
+      <c r="D13" s="47">
+        <v>901310765</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="48">
+        <v>901310765</v>
+      </c>
+      <c r="J13" s="48">
+        <f>$E$6*C13</f>
+        <v>2</v>
+      </c>
+      <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
@@ -1652,38 +1568,37 @@
       <c r="BY13" s="21"/>
       <c r="BZ13" s="21"/>
       <c r="CA13" s="21"/>
-      <c r="CB13" s="21"/>
-    </row>
-    <row r="14" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="48">
+    </row>
+    <row r="14" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="47">
         <v>1</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="49" t="s">
+      <c r="D14" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="48">
+        <v>2535452</v>
+      </c>
+      <c r="H14" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="I14" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="J14" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="K14" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+      <c r="I14" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="48">
+        <f>$E$6*C14</f>
+        <v>1</v>
+      </c>
+      <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
@@ -1752,38 +1667,37 @@
       <c r="BY14" s="21"/>
       <c r="BZ14" s="21"/>
       <c r="CA14" s="21"/>
-      <c r="CB14" s="21"/>
-    </row>
-    <row r="15" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="48">
-        <v>1</v>
-      </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="J15" s="50">
-        <v>22284020</v>
-      </c>
-      <c r="K15" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+    </row>
+    <row r="15" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="47">
+        <v>7</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="48">
+        <f>$E$6*C15</f>
+        <v>7</v>
+      </c>
+      <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
@@ -1852,38 +1766,37 @@
       <c r="BY15" s="21"/>
       <c r="BZ15" s="21"/>
       <c r="CA15" s="21"/>
-      <c r="CB15" s="21"/>
-    </row>
-    <row r="16" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="48">
-        <v>2</v>
-      </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="50">
-        <v>901310765</v>
-      </c>
-      <c r="F16" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="J16" s="50">
-        <v>901310765</v>
-      </c>
-      <c r="K16" s="49">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
+    </row>
+    <row r="16" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="47">
+        <v>4</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="48">
+        <f>$E$6*C16</f>
+        <v>4</v>
+      </c>
+      <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
@@ -1952,38 +1865,37 @@
       <c r="BY16" s="21"/>
       <c r="BZ16" s="21"/>
       <c r="CA16" s="21"/>
-      <c r="CB16" s="21"/>
-    </row>
-    <row r="17" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="48">
-        <v>1</v>
-      </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="49" t="s">
+    </row>
+    <row r="17" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="47">
+        <v>2</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="H17" s="50">
-        <v>2535452</v>
-      </c>
-      <c r="I17" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="J17" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
+      <c r="I17" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" s="48">
+        <f>$E$6*C17</f>
+        <v>2</v>
+      </c>
+      <c r="K17" s="21"/>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
@@ -2052,38 +1964,37 @@
       <c r="BY17" s="21"/>
       <c r="BZ17" s="21"/>
       <c r="CA17" s="21"/>
-      <c r="CB17" s="21"/>
-    </row>
-    <row r="18" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="48">
-        <v>7</v>
-      </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="J18" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="K18" s="49">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
+    </row>
+    <row r="18" spans="1:79" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="47">
+        <v>1</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="48">
+        <f>$E$6*C18</f>
+        <v>1</v>
+      </c>
+      <c r="K18" s="21"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
@@ -2152,453 +2063,50 @@
       <c r="BY18" s="21"/>
       <c r="BZ18" s="21"/>
       <c r="CA18" s="21"/>
-      <c r="CB18" s="21"/>
-    </row>
-    <row r="19" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="48">
-        <v>5</v>
-      </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="I19" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="J19" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="K19" s="49">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="21"/>
-      <c r="AB19" s="21"/>
-      <c r="AC19" s="21"/>
-      <c r="AD19" s="21"/>
-      <c r="AE19" s="21"/>
-      <c r="AF19" s="21"/>
-      <c r="AG19" s="21"/>
-      <c r="AH19" s="21"/>
-      <c r="AI19" s="21"/>
-      <c r="AJ19" s="21"/>
-      <c r="AK19" s="21"/>
-      <c r="AL19" s="21"/>
-      <c r="AM19" s="21"/>
-      <c r="AN19" s="21"/>
-      <c r="AO19" s="21"/>
-      <c r="AP19" s="21"/>
-      <c r="AQ19" s="21"/>
-      <c r="AR19" s="21"/>
-      <c r="AS19" s="21"/>
-      <c r="AT19" s="21"/>
-      <c r="AU19" s="21"/>
-      <c r="AV19" s="21"/>
-      <c r="AW19" s="21"/>
-      <c r="AX19" s="21"/>
-      <c r="AY19" s="21"/>
-      <c r="AZ19" s="21"/>
-      <c r="BA19" s="21"/>
-      <c r="BB19" s="21"/>
-      <c r="BC19" s="21"/>
-      <c r="BD19" s="21"/>
-      <c r="BE19" s="21"/>
-      <c r="BF19" s="21"/>
-      <c r="BG19" s="21"/>
-      <c r="BH19" s="21"/>
-      <c r="BI19" s="21"/>
-      <c r="BJ19" s="21"/>
-      <c r="BK19" s="21"/>
-      <c r="BL19" s="21"/>
-      <c r="BM19" s="21"/>
-      <c r="BN19" s="21"/>
-      <c r="BO19" s="21"/>
-      <c r="BP19" s="21"/>
-      <c r="BQ19" s="21"/>
-      <c r="BR19" s="21"/>
-      <c r="BS19" s="21"/>
-      <c r="BT19" s="21"/>
-      <c r="BU19" s="21"/>
-      <c r="BV19" s="21"/>
-      <c r="BW19" s="21"/>
-      <c r="BX19" s="21"/>
-      <c r="BY19" s="21"/>
-      <c r="BZ19" s="21"/>
-      <c r="CA19" s="21"/>
-      <c r="CB19" s="21"/>
-    </row>
-    <row r="20" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="48">
-        <v>2</v>
-      </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="J20" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="K20" s="49">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="21"/>
-      <c r="AC20" s="21"/>
-      <c r="AD20" s="21"/>
-      <c r="AE20" s="21"/>
-      <c r="AF20" s="21"/>
-      <c r="AG20" s="21"/>
-      <c r="AH20" s="21"/>
-      <c r="AI20" s="21"/>
-      <c r="AJ20" s="21"/>
-      <c r="AK20" s="21"/>
-      <c r="AL20" s="21"/>
-      <c r="AM20" s="21"/>
-      <c r="AN20" s="21"/>
-      <c r="AO20" s="21"/>
-      <c r="AP20" s="21"/>
-      <c r="AQ20" s="21"/>
-      <c r="AR20" s="21"/>
-      <c r="AS20" s="21"/>
-      <c r="AT20" s="21"/>
-      <c r="AU20" s="21"/>
-      <c r="AV20" s="21"/>
-      <c r="AW20" s="21"/>
-      <c r="AX20" s="21"/>
-      <c r="AY20" s="21"/>
-      <c r="AZ20" s="21"/>
-      <c r="BA20" s="21"/>
-      <c r="BB20" s="21"/>
-      <c r="BC20" s="21"/>
-      <c r="BD20" s="21"/>
-      <c r="BE20" s="21"/>
-      <c r="BF20" s="21"/>
-      <c r="BG20" s="21"/>
-      <c r="BH20" s="21"/>
-      <c r="BI20" s="21"/>
-      <c r="BJ20" s="21"/>
-      <c r="BK20" s="21"/>
-      <c r="BL20" s="21"/>
-      <c r="BM20" s="21"/>
-      <c r="BN20" s="21"/>
-      <c r="BO20" s="21"/>
-      <c r="BP20" s="21"/>
-      <c r="BQ20" s="21"/>
-      <c r="BR20" s="21"/>
-      <c r="BS20" s="21"/>
-      <c r="BT20" s="21"/>
-      <c r="BU20" s="21"/>
-      <c r="BV20" s="21"/>
-      <c r="BW20" s="21"/>
-      <c r="BX20" s="21"/>
-      <c r="BY20" s="21"/>
-      <c r="BZ20" s="21"/>
-      <c r="CA20" s="21"/>
-      <c r="CB20" s="21"/>
-    </row>
-    <row r="21" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="48">
-        <v>2</v>
-      </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="J21" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="K21" s="49">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="21"/>
-      <c r="AB21" s="21"/>
-      <c r="AC21" s="21"/>
-      <c r="AD21" s="21"/>
-      <c r="AE21" s="21"/>
-      <c r="AF21" s="21"/>
-      <c r="AG21" s="21"/>
-      <c r="AH21" s="21"/>
-      <c r="AI21" s="21"/>
-      <c r="AJ21" s="21"/>
-      <c r="AK21" s="21"/>
-      <c r="AL21" s="21"/>
-      <c r="AM21" s="21"/>
-      <c r="AN21" s="21"/>
-      <c r="AO21" s="21"/>
-      <c r="AP21" s="21"/>
-      <c r="AQ21" s="21"/>
-      <c r="AR21" s="21"/>
-      <c r="AS21" s="21"/>
-      <c r="AT21" s="21"/>
-      <c r="AU21" s="21"/>
-      <c r="AV21" s="21"/>
-      <c r="AW21" s="21"/>
-      <c r="AX21" s="21"/>
-      <c r="AY21" s="21"/>
-      <c r="AZ21" s="21"/>
-      <c r="BA21" s="21"/>
-      <c r="BB21" s="21"/>
-      <c r="BC21" s="21"/>
-      <c r="BD21" s="21"/>
-      <c r="BE21" s="21"/>
-      <c r="BF21" s="21"/>
-      <c r="BG21" s="21"/>
-      <c r="BH21" s="21"/>
-      <c r="BI21" s="21"/>
-      <c r="BJ21" s="21"/>
-      <c r="BK21" s="21"/>
-      <c r="BL21" s="21"/>
-      <c r="BM21" s="21"/>
-      <c r="BN21" s="21"/>
-      <c r="BO21" s="21"/>
-      <c r="BP21" s="21"/>
-      <c r="BQ21" s="21"/>
-      <c r="BR21" s="21"/>
-      <c r="BS21" s="21"/>
-      <c r="BT21" s="21"/>
-      <c r="BU21" s="21"/>
-      <c r="BV21" s="21"/>
-      <c r="BW21" s="21"/>
-      <c r="BX21" s="21"/>
-      <c r="BY21" s="21"/>
-      <c r="BZ21" s="21"/>
-      <c r="CA21" s="21"/>
-      <c r="CB21" s="21"/>
-    </row>
-    <row r="22" spans="1:80" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="48">
-        <v>1</v>
-      </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="I22" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="J22" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="K22" s="49">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="21"/>
-      <c r="AD22" s="21"/>
-      <c r="AE22" s="21"/>
-      <c r="AF22" s="21"/>
-      <c r="AG22" s="21"/>
-      <c r="AH22" s="21"/>
-      <c r="AI22" s="21"/>
-      <c r="AJ22" s="21"/>
-      <c r="AK22" s="21"/>
-      <c r="AL22" s="21"/>
-      <c r="AM22" s="21"/>
-      <c r="AN22" s="21"/>
-      <c r="AO22" s="21"/>
-      <c r="AP22" s="21"/>
-      <c r="AQ22" s="21"/>
-      <c r="AR22" s="21"/>
-      <c r="AS22" s="21"/>
-      <c r="AT22" s="21"/>
-      <c r="AU22" s="21"/>
-      <c r="AV22" s="21"/>
-      <c r="AW22" s="21"/>
-      <c r="AX22" s="21"/>
-      <c r="AY22" s="21"/>
-      <c r="AZ22" s="21"/>
-      <c r="BA22" s="21"/>
-      <c r="BB22" s="21"/>
-      <c r="BC22" s="21"/>
-      <c r="BD22" s="21"/>
-      <c r="BE22" s="21"/>
-      <c r="BF22" s="21"/>
-      <c r="BG22" s="21"/>
-      <c r="BH22" s="21"/>
-      <c r="BI22" s="21"/>
-      <c r="BJ22" s="21"/>
-      <c r="BK22" s="21"/>
-      <c r="BL22" s="21"/>
-      <c r="BM22" s="21"/>
-      <c r="BN22" s="21"/>
-      <c r="BO22" s="21"/>
-      <c r="BP22" s="21"/>
-      <c r="BQ22" s="21"/>
-      <c r="BR22" s="21"/>
-      <c r="BS22" s="21"/>
-      <c r="BT22" s="21"/>
-      <c r="BU22" s="21"/>
-      <c r="BV22" s="21"/>
-      <c r="BW22" s="21"/>
-      <c r="BX22" s="21"/>
-      <c r="BY22" s="21"/>
-      <c r="BZ22" s="21"/>
-      <c r="CA22" s="21"/>
-      <c r="CB22" s="21"/>
-    </row>
-    <row r="23" spans="1:80" ht="14.65" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="13"/>
-      <c r="C23" s="14">
-        <f>SUM(C11:C22)</f>
-        <v>25</v>
-      </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="1:80" customFormat="1" ht="13.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="E24" s="5" t="s">
+    </row>
+    <row r="19" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="14">
+        <f>SUM(C11:C18)</f>
+        <v>19</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:79" customFormat="1" ht="13.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E20" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:80" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:80" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:80" ht="15.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="9"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="8"/>
+    <row r="21" spans="1:79" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:79" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:79" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2609,4 +2117,10 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>